<commit_message>
Tutorial system additions and fixes
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
   <si>
     <t>Section Text</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Wipe Triggered Objects</t>
   </si>
   <si>
+    <t>Button Blacklist</t>
+  </si>
+  <si>
     <t>Welcome to the Team Management screen!
 Here is where you’ll be dealing with your crew and assigning them their positions for races.
 Before we begin to get into the nitty-gritty of that though, let’s take a look at the three positions you’ll need to fill on your first boat.
@@ -45,6 +48,9 @@
   </si>
   <si>
     <t>PositionUI, ShowPopUp</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>This pop-up provides a short description of the position you just selected, which hopefully will give a small hint on who to pick for the next race once you know all the facts.
@@ -69,6 +75,9 @@
     <t>CrewMemberUI, ShowPopUp</t>
   </si>
   <si>
+    <t>zz Recruit</t>
+  </si>
+  <si>
     <t>This pop-up displays all the details you know on this crew member.
 As you’ve only just started and haven’t spoken to them yet, you know nothing about their skills.
 Also, as far as you’re aware, their opinion of everyone is neutral.
@@ -82,6 +91,9 @@
   </si>
   <si>
     <t>MemberMeetingUI, AskQuestion</t>
+  </si>
+  <si>
+    <t>Fire, close x 2</t>
   </si>
   <si>
     <t>OK, looks like you’ve got the hang of interviewing your team.
@@ -99,14 +111,10 @@
 If you want to remove a crew member from a position, just drag and drop them out of the position.</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>TeamSelectionUI, EnableRacing</t>
   </si>
   <si>
     <t>Happy with where you’ve placed everyone? Click the highlighted button and your current crew will race and you’ll be given clues on what needs improving.
-Don’t worry if you don’t get the perfect crew set-up on the first attempt, there’s four sets of ‘practice’ races before the race proper, and you’ll get feedback on your choices after each.
 Team ratings are based on the crew member’s ratings in the skills needed for the position, their opinion of you, their opinion of everyone else in a position and their current mood.</t>
   </si>
   <si>
@@ -114,6 +122,38 @@
   </si>
   <si>
     <t>TeamSelectionUI, ConfirmLineUp</t>
+  </si>
+  <si>
+    <t>After every race, you'll be given feedback on how your selected crew performed.
+These lights represent how many have been positioned compared to the ideal.
+Hover over each light to see what each number represents.</t>
+  </si>
+  <si>
+    <t>Team Management/Boat Container Bounds/Viewport/Content/Historic Boat 0/Light Container</t>
+  </si>
+  <si>
+    <t>HoverPopUpUI, HoverCheck</t>
+  </si>
+  <si>
+    <t>HoverPopUpUI, HideHover</t>
+  </si>
+  <si>
+    <t>You'll also be given feedback on which areas your team is lacking in (if any).
+Ticks are a sign that you are on the right track to select the ideal team you can.
+The grey question marks meanwhile mean that the information is currently unavilable to you.
+This information is revealed by talking with your team about their skills and relationships further.
+By hovering over each of the blue icons, you can see what areas you need to improve in.</t>
+  </si>
+  <si>
+    <t>Team Management/Boat Container Bounds/Viewport/Content/Historic Boat 0/Icon Container</t>
+  </si>
+  <si>
+    <t>Don’t worry if you don’t get the perfect crew set-up on the first attempt, there’s four sets of ‘practice’ races before the race proper, and you’ll get feedback on your choices after each.</t>
+  </si>
+  <si>
+    <t>PositionUI, ShowPopUp
+CrewMemberUI, ShowPopUp
+PositionUI, LinkCrew</t>
   </si>
   <si>
     <t>OK, time for the race itself!
@@ -156,6 +196,9 @@
     <t>RecruitMemberUI, AskQuestion</t>
   </si>
   <si>
+    <t>Close</t>
+  </si>
+  <si>
     <t>Once you’re happy that you know who you want to hire, simply just click on them to hire them.</t>
   </si>
   <si>
@@ -167,14 +210,6 @@
 Feel free to ask all your team members further questions in interviews as well, if you wish. See you on the other side…</t>
   </si>
   <si>
-    <t>PositionUI, ShowPopUp
-CrewMemberUI, ShowPopUp
-PositionUI, LinkCrew</t>
-  </si>
-  <si>
-    <t>PostRaceEventUI, OnEnable</t>
-  </si>
-  <si>
     <t>Seems that one of your team members is wondering why they weren’t picked for that last race.
 Every so often, events like this will occur after a race, and it’s up to you to handle the situation.
 Click any of the available options to select and say them back to this crew member.</t>
@@ -183,7 +218,7 @@
     <t>Team Management/Pop-up Bounds/Event Pop-Up/Solo</t>
   </si>
   <si>
-    <t>PostRaceEventUI, SendReply</t>
+    <t>PostRaceEventUI, SetBlockerOnClick</t>
   </si>
   <si>
     <t>OK, that’s the conversation finished. To exit and find out what effect this has had, click the highlighted button.</t>
@@ -192,7 +227,10 @@
     <t>Team Management/Pop-up Bounds/Event Pop-Up/Solo/Close</t>
   </si>
   <si>
-    <t>PostRaceEventUI, SetBlockerOnClick</t>
+    <t>PostRaceEventUI, Hide</t>
+  </si>
+  <si>
+    <t>LearningPillUI, ClosePill</t>
   </si>
   <si>
     <t>OK, that's the tutorial finished!
@@ -296,7 +334,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -315,16 +355,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
@@ -335,19 +375,22 @@
       <c r="G2" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
@@ -357,18 +400,21 @@
       </c>
       <c r="G3" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
@@ -378,18 +424,21 @@
       </c>
       <c r="G4" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -399,18 +448,21 @@
       </c>
       <c r="G5" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>1</v>
@@ -420,18 +472,21 @@
       </c>
       <c r="G6" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
@@ -442,19 +497,22 @@
       <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
@@ -465,19 +523,22 @@
       <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
@@ -488,19 +549,22 @@
       <c r="G9" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H9" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
@@ -510,18 +574,21 @@
       </c>
       <c r="G10" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -531,18 +598,21 @@
       </c>
       <c r="G11" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
@@ -552,18 +622,21 @@
       </c>
       <c r="G12" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
@@ -573,18 +646,21 @@
       </c>
       <c r="G13" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>1</v>
@@ -594,18 +670,21 @@
       </c>
       <c r="G14" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -615,18 +694,21 @@
       </c>
       <c r="G15" s="3" t="b">
         <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -637,19 +719,22 @@
       <c r="G16" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="H16" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>0</v>
@@ -660,19 +745,22 @@
       <c r="G17" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H17" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
@@ -683,20 +771,25 @@
       <c r="G18" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H18" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E19" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="3">
         <v>3.0</v>
@@ -704,16 +797,20 @@
       <c r="G19" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H19" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
@@ -724,40 +821,46 @@
       <c r="G20" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H20" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E21" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="3">
-        <v>1.0</v>
+        <v>6.0</v>
       </c>
       <c r="G21" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
@@ -768,19 +871,22 @@
       <c r="G22" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H22" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -791,11 +897,12 @@
       <c r="G23" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H23" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>11</v>
       </c>
@@ -803,30 +910,30 @@
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H24" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>0</v>
@@ -837,36 +944,40 @@
       <c r="G25" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H25" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E26" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G26" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H26" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3" t="b">
         <v>1</v>
@@ -882,6 +993,9 @@
       </c>
       <c r="G27" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28">
@@ -889,13 +1003,13 @@
         <v>41</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -906,17 +1020,22 @@
       <c r="G28" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H28" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="2"/>
+      <c r="A29" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="B29" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C29" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E29" s="3" t="b">
         <v>0</v>
@@ -926,6 +1045,9 @@
       </c>
       <c r="G29" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -936,7 +1058,7 @@
         <v>45</v>
       </c>
       <c r="C30" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>46</v>
@@ -949,6 +1071,9 @@
       </c>
       <c r="G30" s="3" t="b">
         <v>1</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="31">
@@ -959,33 +1084,36 @@
         <v>48</v>
       </c>
       <c r="C31" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E31" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G31" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H31" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C32" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E32" s="3" t="b">
         <v>0</v>
@@ -996,36 +1124,161 @@
       <c r="G32" s="3" t="b">
         <v>1</v>
       </c>
+      <c r="H32" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="A33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G33" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E34" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G34" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G35" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="D36" s="2"/>
+      <c r="A36" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E36" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G37" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="A38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G38" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
@@ -5852,6 +6105,36 @@
       <c r="B1003" s="2"/>
       <c r="D1003" s="2"/>
     </row>
+    <row r="1004">
+      <c r="A1004" s="2"/>
+      <c r="B1004" s="2"/>
+      <c r="D1004" s="2"/>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="2"/>
+      <c r="B1005" s="2"/>
+      <c r="D1005" s="2"/>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="2"/>
+      <c r="B1006" s="2"/>
+      <c r="D1006" s="2"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="2"/>
+      <c r="B1007" s="2"/>
+      <c r="D1007" s="2"/>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="2"/>
+      <c r="B1008" s="2"/>
+      <c r="D1008" s="2"/>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="2"/>
+      <c r="B1009" s="2"/>
+      <c r="D1009" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Functionality to save tutorial progress and allow for tutorial to not be shown added
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
   <si>
     <t>Section Text</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Wipe Triggered Objects</t>
+  </si>
+  <si>
+    <t>Save Progress</t>
   </si>
   <si>
     <t>Button Blacklist</t>
@@ -310,6 +313,7 @@
     <col customWidth="1" min="4" max="4" width="34.57"/>
     <col customWidth="1" min="5" max="5" width="8.0"/>
     <col customWidth="1" min="6" max="6" width="12.29"/>
+    <col customWidth="1" min="8" max="8" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -337,7 +341,9 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -355,16 +361,16 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3" t="b">
         <v>0</v>
@@ -375,22 +381,26 @@
       <c r="G2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
@@ -401,20 +411,24 @@
       <c r="G3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3" t="b">
         <v>1</v>
@@ -425,20 +439,24 @@
       <c r="G4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -449,20 +467,24 @@
       <c r="G5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H5" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3" t="b">
         <v>1</v>
@@ -473,20 +495,24 @@
       <c r="G6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
@@ -497,22 +523,26 @@
       <c r="G7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
@@ -523,22 +553,26 @@
       <c r="G8" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="H8" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
@@ -549,22 +583,26 @@
       <c r="G9" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
@@ -575,20 +613,24 @@
       <c r="G10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -599,20 +641,24 @@
       <c r="G11" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="H11" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
@@ -623,20 +669,24 @@
       <c r="G12" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H12" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
@@ -647,20 +697,24 @@
       <c r="G13" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H13" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>1</v>
@@ -671,20 +725,24 @@
       <c r="G14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="H14" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -695,20 +753,24 @@
       <c r="G15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H15" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -719,22 +781,26 @@
       <c r="G16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H16" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3" t="b">
         <v>0</v>
@@ -745,22 +811,26 @@
       <c r="G17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H17" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E18" s="3" t="b">
         <v>0</v>
@@ -771,22 +841,26 @@
       <c r="G18" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H18" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C19" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E19" s="3" t="b">
         <v>1</v>
@@ -797,20 +871,24 @@
       <c r="G19" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H19" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E20" s="3" t="b">
         <v>0</v>
@@ -821,22 +899,26 @@
       <c r="G20" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H20" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E21" s="3" t="b">
         <v>1</v>
@@ -847,20 +929,24 @@
       <c r="G21" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H21" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3" t="b">
         <v>0</v>
@@ -871,22 +957,26 @@
       <c r="G22" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H22" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" s="3" t="b">
         <v>0</v>
@@ -897,43 +987,52 @@
       <c r="G23" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H23" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H23" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="G24" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H24" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="3"/>
     </row>
     <row r="25">
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="b">
         <v>0</v>
@@ -944,22 +1043,24 @@
       <c r="G25" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H25" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J25" s="3"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E26" s="3" t="b">
         <v>0</v>
@@ -970,20 +1071,26 @@
       <c r="G26" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H26" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J26" s="3"/>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C27" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E27" s="3" t="b">
         <v>0</v>
@@ -994,22 +1101,24 @@
       <c r="G27" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H27" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J27" s="3"/>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -1020,22 +1129,26 @@
       <c r="G28" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H28" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E29" s="3" t="b">
         <v>0</v>
@@ -1046,22 +1159,26 @@
       <c r="G29" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H29" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="E30" s="3" t="b">
         <v>0</v>
@@ -1072,74 +1189,86 @@
       <c r="G30" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H30" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E31" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="G31" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="H31" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E32" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="3">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="G32" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="H32" s="3">
+        <v>-1.0</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E33" s="3" t="b">
         <v>0</v>
@@ -1150,20 +1279,26 @@
       <c r="G33" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H33" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J33" s="3"/>
     </row>
     <row r="34">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="B34" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E34" s="3" t="b">
         <v>0</v>
@@ -1174,22 +1309,24 @@
       <c r="G34" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H34" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J34" s="3"/>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C35" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="E35" s="3" t="b">
         <v>0</v>
@@ -1200,22 +1337,24 @@
       <c r="G35" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H35" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J35" s="3"/>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="C36" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="E36" s="3" t="b">
         <v>0</v>
@@ -1226,20 +1365,26 @@
       <c r="G36" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H36" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="3"/>
     </row>
     <row r="37">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B37" s="1" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -1250,22 +1395,26 @@
       <c r="G37" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H37" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>11</v>
+        <v>59</v>
       </c>
       <c r="C38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="E38" s="3" t="b">
         <v>0</v>
@@ -1276,24 +1425,77 @@
       <c r="G38" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="H38" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J38" s="3"/>
     </row>
     <row r="39">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="D39" s="2"/>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G39" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J39" s="3"/>
     </row>
     <row r="40">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="D40" s="2"/>
+      <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G40" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="D41" s="2"/>
+      <c r="J41" s="3"/>
     </row>
     <row r="42">
       <c r="A42" s="2"/>
@@ -6135,6 +6337,16 @@
       <c r="B1009" s="2"/>
       <c r="D1009" s="2"/>
     </row>
+    <row r="1010">
+      <c r="A1010" s="2"/>
+      <c r="B1010" s="2"/>
+      <c r="D1010" s="2"/>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="2"/>
+      <c r="B1011" s="2"/>
+      <c r="D1011" s="2"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
New Game fixes. Tutorial 'helper' made smaller, functionality to blacklist buttons from use during tutorial added.
</commit_message>
<xml_diff>
--- a/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
+++ b/stm-unity/Assets/Sheets/Sports Team Manager Tutorial.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
   <si>
     <t>Section Text</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>PositionUI, ShowPopUp</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>This pop-up provides a short description of the position you just selected, which hopefully will give a small hint on who to pick for the next race once you know all the facts.
@@ -96,7 +93,9 @@
     <t>MemberMeetingUI, AskQuestion</t>
   </si>
   <si>
-    <t>Fire, close x 2</t>
+    <t>Fire
+Close
+Close (1)</t>
   </si>
   <si>
     <t>OK, looks like you’ve got the hang of interviewing your team.
@@ -112,6 +111,9 @@
     <t>Now you’ve questioned your crew, it’s time to place them in their positions.
 Using the information you’ve gathered from the position descriptions and crew member interviews, place crew members by dragging and dropping them into the position you think they’d best fit.
 If you want to remove a crew member from a position, just drag and drop them out of the position.</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
   <si>
     <t>TeamSelectionUI, EnableRacing</t>
@@ -159,6 +161,10 @@
 PositionUI, LinkCrew</t>
   </si>
   <si>
+    <t>zz Recruit
+Race</t>
+  </si>
+  <si>
     <t>OK, time for the race itself!
 Do you play it safe and pick the best line-up from practice, or try and mix it up when it all matters?
 It’s up to you as their new manager…</t>
@@ -199,13 +205,19 @@
     <t>RecruitMemberUI, AskQuestion</t>
   </si>
   <si>
-    <t>Close</t>
+    <t>Close
+Close (1)
+Button</t>
   </si>
   <si>
     <t>Once you’re happy that you know who you want to hire, simply just click on them to hire them.</t>
   </si>
   <si>
     <t>RecruitMemberUI, Recruit</t>
+  </si>
+  <si>
+    <t>Close
+Close (1)</t>
   </si>
   <si>
     <t>Now we’ve got someone that we feel fits this new position, it’s time to go into the next race session.
@@ -384,23 +396,21 @@
       <c r="H2" s="3">
         <v>2.0</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E3" s="3" t="b">
         <v>0</v>
@@ -414,9 +424,7 @@
       <c r="H3" s="3">
         <v>1.0</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4">
@@ -442,21 +450,19 @@
       <c r="H4" s="3">
         <v>2.0</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E5" s="3" t="b">
         <v>0</v>
@@ -470,9 +476,7 @@
       <c r="H5" s="3">
         <v>1.0</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
     <row r="6">
@@ -498,21 +502,19 @@
       <c r="H6" s="3">
         <v>2.0</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="E7" s="3" t="b">
         <v>0</v>
@@ -526,23 +528,21 @@
       <c r="H7" s="3">
         <v>1.0</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E8" s="3" t="b">
         <v>0</v>
@@ -557,22 +557,22 @@
         <v>0.0</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>0</v>
@@ -587,22 +587,22 @@
         <v>2.0</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>0</v>
@@ -616,21 +616,19 @@
       <c r="H10" s="3">
         <v>1.0</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E11" s="3" t="b">
         <v>1</v>
@@ -645,20 +643,20 @@
         <v>0.0</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E12" s="3" t="b">
         <v>0</v>
@@ -673,20 +671,20 @@
         <v>2.0</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E13" s="3" t="b">
         <v>0</v>
@@ -700,21 +698,19 @@
       <c r="H13" s="3">
         <v>1.0</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="E14" s="3" t="b">
         <v>1</v>
@@ -729,20 +725,20 @@
         <v>0.0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E15" s="3" t="b">
         <v>0</v>
@@ -757,20 +753,20 @@
         <v>2.0</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C16" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E16" s="3" t="b">
         <v>0</v>
@@ -784,17 +780,15 @@
       <c r="H16" s="3">
         <v>1.0</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C17" s="3" t="b">
         <v>0</v>
@@ -815,7 +809,7 @@
         <v>0.0</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J17" s="3"/>
     </row>
@@ -844,9 +838,7 @@
       <c r="H18" s="3">
         <v>1.0</v>
       </c>
-      <c r="I18" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19">
@@ -874,9 +866,7 @@
       <c r="H19" s="3">
         <v>2.0</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
     <row r="20">
@@ -902,9 +892,7 @@
       <c r="H20" s="3">
         <v>1.0</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
     <row r="21">
@@ -932,9 +920,7 @@
       <c r="H21" s="3">
         <v>2.0</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
     <row r="22">
@@ -960,9 +946,7 @@
       <c r="H22" s="3">
         <v>1.0</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23">
@@ -970,7 +954,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>1</v>
@@ -991,14 +975,14 @@
         <v>1.0</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="J23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>1</v>
@@ -1019,14 +1003,14 @@
         <v>1.0</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J24" s="3"/>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="b">
         <v>1</v>
@@ -1047,14 +1031,14 @@
         <v>1.0</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J25" s="3"/>
     </row>
     <row r="26">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C26" s="3" t="b">
         <v>1</v>
@@ -1075,16 +1059,16 @@
         <v>1.0</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J26" s="3"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C27" s="3" t="b">
         <v>1</v>
@@ -1105,20 +1089,20 @@
         <v>2.0</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J27" s="3"/>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C28" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E28" s="3" t="b">
         <v>0</v>
@@ -1133,16 +1117,16 @@
         <v>1.0</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="J28" s="3"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>1</v>
@@ -1162,23 +1146,21 @@
       <c r="H29" s="3">
         <v>2.0</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="3" t="b">
         <v>0</v>
@@ -1192,23 +1174,21 @@
       <c r="H30" s="3">
         <v>1.0</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E31" s="3" t="b">
         <v>0</v>
@@ -1222,23 +1202,21 @@
       <c r="H31" s="3">
         <v>0.0</v>
       </c>
-      <c r="I31" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I31" s="3"/>
       <c r="J31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="b">
         <v>1</v>
@@ -1253,22 +1231,22 @@
         <v>-1.0</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E33" s="3" t="b">
         <v>0</v>
@@ -1283,16 +1261,16 @@
         <v>1.0</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J33" s="3"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C34" s="3" t="b">
         <v>1</v>
@@ -1312,15 +1290,13 @@
       <c r="H34" s="3">
         <v>1.0</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I34" s="3"/>
       <c r="J34" s="3"/>
     </row>
     <row r="35">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C35" s="3" t="b">
         <v>1</v>
@@ -1340,21 +1316,19 @@
       <c r="H35" s="3">
         <v>2.0</v>
       </c>
-      <c r="I35" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I35" s="3"/>
       <c r="J35" s="3"/>
     </row>
     <row r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C36" s="3" t="b">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E36" s="3" t="b">
         <v>0</v>
@@ -1368,23 +1342,21 @@
       <c r="H36" s="3">
         <v>1.0</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E37" s="3" t="b">
         <v>0</v>
@@ -1398,23 +1370,21 @@
       <c r="H37" s="3">
         <v>3.0</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C38" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E38" s="3" t="b">
         <v>0</v>
@@ -1428,21 +1398,19 @@
       <c r="H38" s="3">
         <v>2.0</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I38" s="3"/>
       <c r="J38" s="3"/>
     </row>
     <row r="39">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E39" s="3" t="b">
         <v>0</v>
@@ -1456,17 +1424,15 @@
       <c r="H39" s="3">
         <v>1.0</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I39" s="3"/>
       <c r="J39" s="3"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>0</v>
@@ -1486,9 +1452,7 @@
       <c r="H40" s="3">
         <v>1.0</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
     <row r="41">

</xml_diff>